<commit_message>
[Overall Qual, Gr Liv Area]
</commit_message>
<xml_diff>
--- a/Courses/Courses/course_projects/Data/module_3/meta_data.xlsx
+++ b/Courses/Courses/course_projects/Data/module_3/meta_data.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="581">
   <si>
     <t>1-STORY 1946 &amp; NEWER ALL STYLES</t>
   </si>
@@ -1424,9 +1424,6 @@
     <t>Roof material</t>
   </si>
   <si>
-    <t>Exterior 1</t>
-  </si>
-  <si>
     <t>Exterior covering on house</t>
   </si>
   <si>
@@ -1571,9 +1568,6 @@
     <t>Kitchen</t>
   </si>
   <si>
-    <t xml:space="preserve">KitchenQual </t>
-  </si>
-  <si>
     <t>Kitchen quality</t>
   </si>
   <si>
@@ -1736,9 +1730,6 @@
     <t>Overall Cond</t>
   </si>
   <si>
-    <t>HeatingQC</t>
-  </si>
-  <si>
     <t>Functional</t>
   </si>
   <si>
@@ -1757,10 +1748,19 @@
     <t>Bldg Type</t>
   </si>
   <si>
-    <t>Exterior 2</t>
-  </si>
-  <si>
     <t>Sale Condition</t>
+  </si>
+  <si>
+    <t>Kitchen Qual</t>
+  </si>
+  <si>
+    <t>Exterior 1st</t>
+  </si>
+  <si>
+    <t>Exterior 2nd</t>
+  </si>
+  <si>
+    <t>Heating QC</t>
   </si>
 </sst>
 </file>
@@ -2130,11 +2130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A332" sqref="A332"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="A246" sqref="A246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,10 +2160,10 @@
         <v>425</v>
       </c>
       <c r="E1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2195,7 +2194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>30</v>
       </c>
@@ -2203,7 +2202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>40</v>
       </c>
@@ -2211,7 +2210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>45</v>
       </c>
@@ -2219,7 +2218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>50</v>
       </c>
@@ -2227,7 +2226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>60</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>70</v>
       </c>
@@ -2243,7 +2242,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>75</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>80</v>
       </c>
@@ -2259,7 +2258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>85</v>
       </c>
@@ -2267,7 +2266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>90</v>
       </c>
@@ -2275,7 +2274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>120</v>
       </c>
@@ -2283,7 +2282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>150</v>
       </c>
@@ -2291,7 +2290,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>160</v>
       </c>
@@ -2299,7 +2298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>180</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>190</v>
       </c>
@@ -2317,7 +2316,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B19" t="s">
         <v>426</v>
@@ -2332,7 +2331,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>17</v>
       </c>
@@ -2340,7 +2339,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>19</v>
       </c>
@@ -2348,7 +2347,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>21</v>
       </c>
@@ -2356,7 +2355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>23</v>
       </c>
@@ -2364,7 +2363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>25</v>
       </c>
@@ -2372,7 +2371,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>27</v>
       </c>
@@ -2380,7 +2379,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>29</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>428</v>
       </c>
@@ -2399,7 +2398,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>431</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>33</v>
       </c>
@@ -2452,7 +2451,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>33</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>35</v>
       </c>
@@ -2468,7 +2467,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>439</v>
       </c>
@@ -2488,7 +2487,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>39</v>
       </c>
@@ -2499,7 +2498,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>41</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>43</v>
       </c>
@@ -2538,7 +2537,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>47</v>
       </c>
@@ -2546,7 +2545,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>49</v>
       </c>
@@ -2554,7 +2553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>51</v>
       </c>
@@ -2562,7 +2561,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>442</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>55</v>
       </c>
@@ -2593,7 +2592,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>57</v>
       </c>
@@ -2604,7 +2603,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>59</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>63</v>
       </c>
@@ -2640,7 +2639,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>65</v>
       </c>
@@ -2648,7 +2647,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>67</v>
       </c>
@@ -2656,7 +2655,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>69</v>
       </c>
@@ -2664,7 +2663,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>446</v>
       </c>
@@ -2684,7 +2683,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>73</v>
       </c>
@@ -2695,7 +2694,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>75</v>
       </c>
@@ -2723,7 +2722,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>79</v>
       </c>
@@ -2731,7 +2730,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>81</v>
       </c>
@@ -2739,7 +2738,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>83</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>85</v>
       </c>
@@ -2755,7 +2754,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>87</v>
       </c>
@@ -2763,7 +2762,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>89</v>
       </c>
@@ -2771,7 +2770,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>91</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>93</v>
       </c>
@@ -2787,7 +2786,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>95</v>
       </c>
@@ -2795,7 +2794,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>97</v>
       </c>
@@ -2803,7 +2802,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="65" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>99</v>
       </c>
@@ -2811,7 +2810,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>101</v>
       </c>
@@ -2819,7 +2818,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>103</v>
       </c>
@@ -2827,7 +2826,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>105</v>
       </c>
@@ -2835,7 +2834,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>107</v>
       </c>
@@ -2843,7 +2842,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>109</v>
       </c>
@@ -2851,7 +2850,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
         <v>111</v>
       </c>
@@ -2859,7 +2858,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>113</v>
       </c>
@@ -2867,7 +2866,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>115</v>
       </c>
@@ -2875,7 +2874,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
         <v>117</v>
       </c>
@@ -2883,7 +2882,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="75" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>119</v>
       </c>
@@ -2891,7 +2890,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="76" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
         <v>121</v>
       </c>
@@ -2899,7 +2898,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="77" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
         <v>123</v>
       </c>
@@ -2907,7 +2906,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="78" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
         <v>125</v>
       </c>
@@ -2915,7 +2914,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="79" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
         <v>127</v>
       </c>
@@ -2923,7 +2922,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="4:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
         <v>129</v>
       </c>
@@ -2931,7 +2930,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
         <v>131</v>
       </c>
@@ -2956,7 +2955,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
         <v>135</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D84" t="s">
         <v>137</v>
       </c>
@@ -2972,7 +2971,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
         <v>139</v>
       </c>
@@ -2980,7 +2979,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D86" t="s">
         <v>141</v>
       </c>
@@ -2988,7 +2987,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
         <v>143</v>
       </c>
@@ -2996,7 +2995,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
         <v>145</v>
       </c>
@@ -3004,7 +3003,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D89" t="s">
         <v>147</v>
       </c>
@@ -3012,7 +3011,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D90" t="s">
         <v>149</v>
       </c>
@@ -3037,7 +3036,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D92" t="s">
         <v>135</v>
       </c>
@@ -3045,7 +3044,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D93" t="s">
         <v>137</v>
       </c>
@@ -3053,7 +3052,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D94" t="s">
         <v>139</v>
       </c>
@@ -3061,7 +3060,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D95" t="s">
         <v>141</v>
       </c>
@@ -3069,7 +3068,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D96" t="s">
         <v>143</v>
       </c>
@@ -3077,7 +3076,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
         <v>145</v>
       </c>
@@ -3085,7 +3084,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D98" t="s">
         <v>147</v>
       </c>
@@ -3093,7 +3092,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
         <v>149</v>
       </c>
@@ -3103,7 +3102,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B100" t="s">
         <v>454</v>
@@ -3118,7 +3117,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D101" t="s">
         <v>153</v>
       </c>
@@ -3126,7 +3125,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" t="s">
         <v>155</v>
       </c>
@@ -3134,7 +3133,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
         <v>157</v>
       </c>
@@ -3142,7 +3141,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
         <v>159</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D106" t="s">
         <v>163</v>
       </c>
@@ -3175,7 +3174,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
         <v>165</v>
       </c>
@@ -3183,7 +3182,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
         <v>167</v>
       </c>
@@ -3191,7 +3190,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
         <v>169</v>
       </c>
@@ -3199,7 +3198,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
         <v>171</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D111" t="s">
         <v>173</v>
       </c>
@@ -3215,7 +3214,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D112" t="s">
         <v>175</v>
       </c>
@@ -3223,7 +3222,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>457</v>
       </c>
@@ -3243,7 +3242,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D114">
         <v>9</v>
       </c>
@@ -3254,7 +3253,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D115">
         <v>8</v>
       </c>
@@ -3265,7 +3264,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D116">
         <v>7</v>
       </c>
@@ -3276,7 +3275,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D117">
         <v>6</v>
       </c>
@@ -3287,7 +3286,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D118">
         <v>5</v>
       </c>
@@ -3298,7 +3297,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D119">
         <v>4</v>
       </c>
@@ -3309,7 +3308,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D120">
         <v>3</v>
       </c>
@@ -3320,7 +3319,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D121">
         <v>2</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D122">
         <v>1</v>
       </c>
@@ -3342,9 +3341,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B123" t="s">
         <v>459</v>
@@ -3362,7 +3361,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D124">
         <v>9</v>
       </c>
@@ -3373,7 +3372,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D125">
         <v>8</v>
       </c>
@@ -3384,7 +3383,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D126">
         <v>7</v>
       </c>
@@ -3395,7 +3394,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D127">
         <v>6</v>
       </c>
@@ -3406,7 +3405,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D128">
         <v>5</v>
       </c>
@@ -3417,7 +3416,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D129">
         <v>4</v>
       </c>
@@ -3428,7 +3427,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D130">
         <v>3</v>
       </c>
@@ -3439,7 +3438,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D131">
         <v>2</v>
       </c>
@@ -3450,7 +3449,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D132">
         <v>1</v>
       </c>
@@ -3461,7 +3460,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>460</v>
       </c>
@@ -3472,9 +3471,9 @@
         <v>462</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B134" t="s">
         <v>463</v>
@@ -3500,7 +3499,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D136" t="s">
         <v>189</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
         <v>191</v>
       </c>
@@ -3516,7 +3515,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
         <v>193</v>
       </c>
@@ -3524,7 +3523,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
         <v>195</v>
       </c>
@@ -3532,7 +3531,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
         <v>197</v>
       </c>
@@ -3557,7 +3556,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D142" t="s">
         <v>201</v>
       </c>
@@ -3565,7 +3564,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
         <v>203</v>
       </c>
@@ -3573,7 +3572,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D144" t="s">
         <v>205</v>
       </c>
@@ -3581,7 +3580,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D145" t="s">
         <v>207</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D146" t="s">
         <v>209</v>
       </c>
@@ -3597,7 +3596,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
         <v>211</v>
       </c>
@@ -3605,7 +3604,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
         <v>213</v>
       </c>
@@ -3615,10 +3614,10 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>578</v>
+      </c>
+      <c r="B149" t="s">
         <v>468</v>
-      </c>
-      <c r="B149" t="s">
-        <v>469</v>
       </c>
       <c r="C149" t="s">
         <v>420</v>
@@ -3630,7 +3629,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D150" t="s">
         <v>217</v>
       </c>
@@ -3638,7 +3637,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
         <v>219</v>
       </c>
@@ -3646,7 +3645,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
         <v>221</v>
       </c>
@@ -3654,7 +3653,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
         <v>223</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
         <v>225</v>
       </c>
@@ -3670,7 +3669,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
         <v>227</v>
       </c>
@@ -3678,7 +3677,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
         <v>229</v>
       </c>
@@ -3686,7 +3685,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
         <v>231</v>
       </c>
@@ -3694,7 +3693,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D158" t="s">
         <v>233</v>
       </c>
@@ -3702,7 +3701,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D159" t="s">
         <v>235</v>
       </c>
@@ -3710,7 +3709,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D160" t="s">
         <v>237</v>
       </c>
@@ -3718,7 +3717,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D161" t="s">
         <v>239</v>
       </c>
@@ -3726,7 +3725,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
         <v>241</v>
       </c>
@@ -3734,7 +3733,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
         <v>243</v>
       </c>
@@ -3742,7 +3741,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D164" t="s">
         <v>245</v>
       </c>
@@ -3750,7 +3749,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D165" t="s">
         <v>247</v>
       </c>
@@ -3763,7 +3762,7 @@
         <v>579</v>
       </c>
       <c r="B166" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C166" t="s">
         <v>420</v>
@@ -3775,7 +3774,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D167" t="s">
         <v>217</v>
       </c>
@@ -3783,7 +3782,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
         <v>219</v>
       </c>
@@ -3791,7 +3790,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D169" t="s">
         <v>221</v>
       </c>
@@ -3799,7 +3798,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D170" t="s">
         <v>223</v>
       </c>
@@ -3807,7 +3806,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D171" t="s">
         <v>225</v>
       </c>
@@ -3815,7 +3814,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D172" t="s">
         <v>227</v>
       </c>
@@ -3823,7 +3822,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D173" t="s">
         <v>229</v>
       </c>
@@ -3831,7 +3830,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D174" t="s">
         <v>231</v>
       </c>
@@ -3839,7 +3838,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D175" t="s">
         <v>233</v>
       </c>
@@ -3847,7 +3846,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D176" t="s">
         <v>235</v>
       </c>
@@ -3855,7 +3854,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D177" t="s">
         <v>237</v>
       </c>
@@ -3863,7 +3862,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D178" t="s">
         <v>239</v>
       </c>
@@ -3871,7 +3870,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D179" t="s">
         <v>241</v>
       </c>
@@ -3879,7 +3878,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
         <v>243</v>
       </c>
@@ -3887,7 +3886,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
         <v>245</v>
       </c>
@@ -3895,7 +3894,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D182" t="s">
         <v>247</v>
       </c>
@@ -3905,10 +3904,10 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>470</v>
+      </c>
+      <c r="B183" t="s">
         <v>471</v>
-      </c>
-      <c r="B183" t="s">
-        <v>472</v>
       </c>
       <c r="C183" t="s">
         <v>420</v>
@@ -3920,7 +3919,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D184" t="s">
         <v>221</v>
       </c>
@@ -3928,7 +3927,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D185" t="s">
         <v>223</v>
       </c>
@@ -3936,7 +3935,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D186" t="s">
         <v>249</v>
       </c>
@@ -3944,7 +3943,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
         <v>239</v>
       </c>
@@ -3952,23 +3951,23 @@
         <v>240</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>472</v>
+      </c>
+      <c r="B188" t="s">
         <v>473</v>
-      </c>
-      <c r="B188" t="s">
-        <v>474</v>
       </c>
       <c r="C188" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>474</v>
+      </c>
+      <c r="B189" t="s">
         <v>475</v>
-      </c>
-      <c r="B189" t="s">
-        <v>476</v>
       </c>
       <c r="C189" t="s">
         <v>437</v>
@@ -3983,7 +3982,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D190" t="s">
         <v>252</v>
       </c>
@@ -3994,7 +3993,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D191" t="s">
         <v>253</v>
       </c>
@@ -4005,7 +4004,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D192" t="s">
         <v>255</v>
       </c>
@@ -4016,7 +4015,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D193" t="s">
         <v>256</v>
       </c>
@@ -4027,12 +4026,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>476</v>
+      </c>
+      <c r="B194" t="s">
         <v>477</v>
-      </c>
-      <c r="B194" t="s">
-        <v>478</v>
       </c>
       <c r="C194" t="s">
         <v>437</v>
@@ -4047,7 +4046,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D195" t="s">
         <v>252</v>
       </c>
@@ -4058,7 +4057,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D196" t="s">
         <v>253</v>
       </c>
@@ -4069,7 +4068,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D197" t="s">
         <v>255</v>
       </c>
@@ -4080,7 +4079,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D198" t="s">
         <v>256</v>
       </c>
@@ -4093,10 +4092,10 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>478</v>
+      </c>
+      <c r="B199" t="s">
         <v>479</v>
-      </c>
-      <c r="B199" t="s">
-        <v>480</v>
       </c>
       <c r="C199" t="s">
         <v>420</v>
@@ -4111,7 +4110,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
         <v>223</v>
       </c>
@@ -4122,7 +4121,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
         <v>259</v>
       </c>
@@ -4133,7 +4132,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D202" t="s">
         <v>261</v>
       </c>
@@ -4144,7 +4143,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D203" t="s">
         <v>239</v>
       </c>
@@ -4155,7 +4154,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D204" t="s">
         <v>263</v>
       </c>
@@ -4166,12 +4165,12 @@
         <v>264</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>480</v>
+      </c>
+      <c r="B205" t="s">
         <v>481</v>
-      </c>
-      <c r="B205" t="s">
-        <v>482</v>
       </c>
       <c r="C205" t="s">
         <v>437</v>
@@ -4186,7 +4185,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D206" t="s">
         <v>252</v>
       </c>
@@ -4197,7 +4196,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D207" t="s">
         <v>253</v>
       </c>
@@ -4208,7 +4207,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D208" t="s">
         <v>255</v>
       </c>
@@ -4219,7 +4218,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D209" t="s">
         <v>256</v>
       </c>
@@ -4230,7 +4229,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D210" t="s">
         <v>270</v>
       </c>
@@ -4241,12 +4240,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>482</v>
+      </c>
+      <c r="B211" t="s">
         <v>483</v>
-      </c>
-      <c r="B211" t="s">
-        <v>484</v>
       </c>
       <c r="C211" t="s">
         <v>437</v>
@@ -4261,7 +4260,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D212" t="s">
         <v>252</v>
       </c>
@@ -4272,7 +4271,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D213" t="s">
         <v>253</v>
       </c>
@@ -4283,7 +4282,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D214" t="s">
         <v>255</v>
       </c>
@@ -4294,7 +4293,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
         <v>256</v>
       </c>
@@ -4305,7 +4304,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D216" t="s">
         <v>270</v>
       </c>
@@ -4316,12 +4315,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>275</v>
       </c>
       <c r="B217" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C217" t="s">
         <v>437</v>
@@ -4336,7 +4335,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D218" t="s">
         <v>277</v>
       </c>
@@ -4347,7 +4346,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D219" t="s">
         <v>279</v>
       </c>
@@ -4358,7 +4357,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D220" t="s">
         <v>281</v>
       </c>
@@ -4369,7 +4368,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D221" t="s">
         <v>270</v>
       </c>
@@ -4380,12 +4379,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>283</v>
       </c>
       <c r="B222" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C222" t="s">
         <v>437</v>
@@ -4400,7 +4399,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D223" t="s">
         <v>286</v>
       </c>
@@ -4411,7 +4410,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D224" t="s">
         <v>288</v>
       </c>
@@ -4422,7 +4421,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D225" t="s">
         <v>290</v>
       </c>
@@ -4433,7 +4432,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D226" t="s">
         <v>292</v>
       </c>
@@ -4444,7 +4443,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D227" t="s">
         <v>294</v>
       </c>
@@ -4455,7 +4454,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D228" t="s">
         <v>270</v>
       </c>
@@ -4466,23 +4465,23 @@
         <v>271</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B229" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C229" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>296</v>
       </c>
       <c r="B230" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C230" t="s">
         <v>437</v>
@@ -4497,7 +4496,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D231" t="s">
         <v>286</v>
       </c>
@@ -4508,7 +4507,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D232" t="s">
         <v>288</v>
       </c>
@@ -4519,7 +4518,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D233" t="s">
         <v>290</v>
       </c>
@@ -4530,7 +4529,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D234" t="s">
         <v>292</v>
       </c>
@@ -4541,7 +4540,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D235" t="s">
         <v>294</v>
       </c>
@@ -4552,7 +4551,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D236" t="s">
         <v>270</v>
       </c>
@@ -4563,34 +4562,34 @@
         <v>271</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
+        <v>488</v>
+      </c>
+      <c r="B237" t="s">
         <v>489</v>
-      </c>
-      <c r="B237" t="s">
-        <v>490</v>
       </c>
       <c r="C237" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
+        <v>490</v>
+      </c>
+      <c r="B238" t="s">
         <v>491</v>
-      </c>
-      <c r="B238" t="s">
-        <v>492</v>
       </c>
       <c r="C238" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
+        <v>492</v>
+      </c>
+      <c r="B239" t="s">
         <v>493</v>
-      </c>
-      <c r="B239" t="s">
-        <v>494</v>
       </c>
       <c r="C239" t="s">
         <v>430</v>
@@ -4601,7 +4600,7 @@
         <v>297</v>
       </c>
       <c r="B240" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C240" t="s">
         <v>420</v>
@@ -4613,7 +4612,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D241" t="s">
         <v>300</v>
       </c>
@@ -4621,7 +4620,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D242" t="s">
         <v>302</v>
       </c>
@@ -4629,7 +4628,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D243" t="s">
         <v>304</v>
       </c>
@@ -4637,7 +4636,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D244" t="s">
         <v>306</v>
       </c>
@@ -4645,7 +4644,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D245" t="s">
         <v>308</v>
       </c>
@@ -4653,12 +4652,12 @@
         <v>309</v>
       </c>
     </row>
-    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
       <c r="B246" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C246" t="s">
         <v>437</v>
@@ -4673,7 +4672,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D247" t="s">
         <v>252</v>
       </c>
@@ -4684,7 +4683,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D248" t="s">
         <v>253</v>
       </c>
@@ -4695,7 +4694,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D249" t="s">
         <v>255</v>
       </c>
@@ -4706,7 +4705,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D250" t="s">
         <v>256</v>
       </c>
@@ -4719,10 +4718,10 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
+        <v>496</v>
+      </c>
+      <c r="B251" t="s">
         <v>497</v>
-      </c>
-      <c r="B251" t="s">
-        <v>498</v>
       </c>
       <c r="C251" t="s">
         <v>420</v>
@@ -4734,7 +4733,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D252" t="s">
         <v>312</v>
       </c>
@@ -4742,12 +4741,12 @@
         <v>313</v>
       </c>
     </row>
-    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
+        <v>498</v>
+      </c>
+      <c r="B253" t="s">
         <v>499</v>
-      </c>
-      <c r="B253" t="s">
-        <v>500</v>
       </c>
       <c r="C253" t="s">
         <v>437</v>
@@ -4762,7 +4761,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D254" t="s">
         <v>316</v>
       </c>
@@ -4773,7 +4772,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D255" t="s">
         <v>318</v>
       </c>
@@ -4784,7 +4783,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D256" t="s">
         <v>320</v>
       </c>
@@ -4795,7 +4794,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D257" t="s">
         <v>322</v>
       </c>
@@ -4806,168 +4805,186 @@
         <v>323</v>
       </c>
     </row>
-    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
+        <v>500</v>
+      </c>
+      <c r="B258" t="s">
         <v>501</v>
-      </c>
-      <c r="B258" t="s">
-        <v>502</v>
       </c>
       <c r="C258" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
+        <v>502</v>
+      </c>
+      <c r="B259" t="s">
         <v>503</v>
-      </c>
-      <c r="B259" t="s">
-        <v>504</v>
       </c>
       <c r="C259" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B260" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C260" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B261" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C261" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B262" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C262" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B263" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C263" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B264" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C264" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B265" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C265" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B266" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C266" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>517</v>
+        <v>577</v>
       </c>
       <c r="B267" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C267" t="s">
+        <v>437</v>
+      </c>
+      <c r="D267" t="s">
         <v>251</v>
       </c>
-      <c r="D267" t="s">
+      <c r="E267">
+        <v>10</v>
+      </c>
+      <c r="F267" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C268" t="s">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D268" t="s">
         <v>252</v>
       </c>
-      <c r="D268" t="s">
+      <c r="E268">
+        <v>8</v>
+      </c>
+      <c r="F268" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C269" t="s">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D269" t="s">
         <v>253</v>
       </c>
-      <c r="D269" t="s">
+      <c r="E269">
+        <v>6</v>
+      </c>
+      <c r="F269" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C270" t="s">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D270" t="s">
         <v>255</v>
       </c>
-      <c r="D270" t="s">
+      <c r="E270">
+        <v>4</v>
+      </c>
+      <c r="F270" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C271" t="s">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D271" t="s">
         <v>256</v>
       </c>
-      <c r="D271" t="s">
+      <c r="E271">
+        <v>0</v>
+      </c>
+      <c r="F271" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>325</v>
       </c>
       <c r="B272" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C272" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B273" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C273" t="s">
         <v>437</v>
@@ -4982,7 +4999,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D274" t="s">
         <v>328</v>
       </c>
@@ -4993,7 +5010,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D275" t="s">
         <v>330</v>
       </c>
@@ -5004,7 +5021,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D276" t="s">
         <v>73</v>
       </c>
@@ -5015,7 +5032,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D277" t="s">
         <v>333</v>
       </c>
@@ -5026,7 +5043,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D278" t="s">
         <v>335</v>
       </c>
@@ -5037,7 +5054,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D279" t="s">
         <v>75</v>
       </c>
@@ -5048,7 +5065,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D280" t="s">
         <v>338</v>
       </c>
@@ -5059,23 +5076,23 @@
         <v>339</v>
       </c>
     </row>
-    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B281" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C281" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B282" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C282" t="s">
         <v>437</v>
@@ -5090,7 +5107,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D283" t="s">
         <v>252</v>
       </c>
@@ -5101,7 +5118,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D284" t="s">
         <v>253</v>
       </c>
@@ -5112,7 +5129,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D285" t="s">
         <v>255</v>
       </c>
@@ -5123,7 +5140,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D286" t="s">
         <v>256</v>
       </c>
@@ -5134,7 +5151,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D287" t="s">
         <v>270</v>
       </c>
@@ -5147,10 +5164,10 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B288" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C288" t="s">
         <v>420</v>
@@ -5162,7 +5179,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D289" t="s">
         <v>348</v>
       </c>
@@ -5170,7 +5187,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D290" t="s">
         <v>350</v>
       </c>
@@ -5178,7 +5195,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D291" t="s">
         <v>352</v>
       </c>
@@ -5186,7 +5203,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D292" t="s">
         <v>354</v>
       </c>
@@ -5194,7 +5211,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D293" t="s">
         <v>356</v>
       </c>
@@ -5202,7 +5219,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D294" t="s">
         <v>270</v>
       </c>
@@ -5210,23 +5227,23 @@
         <v>358</v>
       </c>
     </row>
-    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B295" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C295" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B296" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C296" t="s">
         <v>437</v>
@@ -5241,7 +5258,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D297" t="s">
         <v>361</v>
       </c>
@@ -5252,7 +5269,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D298" t="s">
         <v>294</v>
       </c>
@@ -5263,7 +5280,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D299" t="s">
         <v>270</v>
       </c>
@@ -5274,34 +5291,34 @@
         <v>358</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B300" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C300" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B301" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C301" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B302" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C302" t="s">
         <v>437</v>
@@ -5316,7 +5333,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D303" t="s">
         <v>252</v>
       </c>
@@ -5327,7 +5344,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D304" t="s">
         <v>253</v>
       </c>
@@ -5338,7 +5355,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D305" t="s">
         <v>255</v>
       </c>
@@ -5349,7 +5366,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D306" t="s">
         <v>256</v>
       </c>
@@ -5360,7 +5377,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D307" t="s">
         <v>270</v>
       </c>
@@ -5371,12 +5388,12 @@
         <v>358</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B308" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C308" t="s">
         <v>437</v>
@@ -5391,7 +5408,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D309" t="s">
         <v>252</v>
       </c>
@@ -5402,7 +5419,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D310" t="s">
         <v>253</v>
       </c>
@@ -5413,7 +5430,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D311" t="s">
         <v>255</v>
       </c>
@@ -5424,7 +5441,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D312" t="s">
         <v>256</v>
       </c>
@@ -5435,7 +5452,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D313" t="s">
         <v>270</v>
       </c>
@@ -5446,12 +5463,12 @@
         <v>358</v>
       </c>
     </row>
-    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B314" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C314" t="s">
         <v>437</v>
@@ -5466,7 +5483,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D315" t="s">
         <v>365</v>
       </c>
@@ -5477,7 +5494,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D316" t="s">
         <v>310</v>
       </c>
@@ -5488,67 +5505,67 @@
         <v>367</v>
       </c>
     </row>
-    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B317" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C317" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B318" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C318" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B319" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C319" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B320" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C320" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B321" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C321" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B322" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C322" t="s">
         <v>437</v>
@@ -5563,7 +5580,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D323" t="s">
         <v>252</v>
       </c>
@@ -5574,7 +5591,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D324" t="s">
         <v>253</v>
       </c>
@@ -5585,7 +5602,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D325" t="s">
         <v>255</v>
       </c>
@@ -5596,7 +5613,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D326" t="s">
         <v>270</v>
       </c>
@@ -5607,12 +5624,12 @@
         <v>368</v>
       </c>
     </row>
-    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B327" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C327" t="s">
         <v>437</v>
@@ -5627,7 +5644,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D328" t="s">
         <v>371</v>
       </c>
@@ -5638,7 +5655,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D329" t="s">
         <v>373</v>
       </c>
@@ -5649,7 +5666,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D330" t="s">
         <v>375</v>
       </c>
@@ -5660,7 +5677,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D331" t="s">
         <v>270</v>
       </c>
@@ -5673,10 +5690,10 @@
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B332" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C332" t="s">
         <v>420</v>
@@ -5688,7 +5705,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D333" t="s">
         <v>380</v>
       </c>
@@ -5696,7 +5713,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D334" t="s">
         <v>382</v>
       </c>
@@ -5704,7 +5721,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D335" t="s">
         <v>197</v>
       </c>
@@ -5712,7 +5729,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D336" t="s">
         <v>384</v>
       </c>
@@ -5720,7 +5737,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D337" t="s">
         <v>270</v>
       </c>
@@ -5728,34 +5745,34 @@
         <v>250</v>
       </c>
     </row>
-    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B338" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C338" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B339" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C339" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B340" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C340" t="s">
         <v>462</v>
@@ -5763,10 +5780,10 @@
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B341" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C341" t="s">
         <v>420</v>
@@ -5781,7 +5798,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D342" t="s">
         <v>388</v>
       </c>
@@ -5792,7 +5809,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D343" t="s">
         <v>390</v>
       </c>
@@ -5803,7 +5820,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D344" t="s">
         <v>392</v>
       </c>
@@ -5814,7 +5831,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D345" t="s">
         <v>394</v>
       </c>
@@ -5825,7 +5842,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D346" t="s">
         <v>396</v>
       </c>
@@ -5836,7 +5853,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D347" t="s">
         <v>398</v>
       </c>
@@ -5847,7 +5864,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D348" t="s">
         <v>400</v>
       </c>
@@ -5858,7 +5875,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D349" t="s">
         <v>402</v>
       </c>
@@ -5869,7 +5886,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D350" t="s">
         <v>404</v>
       </c>
@@ -5882,10 +5899,10 @@
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B351" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C351" t="s">
         <v>420</v>
@@ -5897,7 +5914,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D352" t="s">
         <v>407</v>
       </c>
@@ -5905,7 +5922,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D353" t="s">
         <v>409</v>
       </c>
@@ -5913,7 +5930,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D354" t="s">
         <v>411</v>
       </c>
@@ -5921,7 +5938,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D355" t="s">
         <v>413</v>
       </c>
@@ -5929,7 +5946,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D356" t="s">
         <v>415</v>
       </c>
@@ -5937,25 +5954,19 @@
         <v>416</v>
       </c>
     </row>
-    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B357" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C357" t="s">
         <v>430</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F357">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Nominal"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F357"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add features to complex model
</commit_message>
<xml_diff>
--- a/Courses/Courses/course_projects/Data/module_3/meta_data.xlsx
+++ b/Courses/Courses/course_projects/Data/module_3/meta_data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{735A848A-67B9-4B3D-9E53-0FBF4BCCD8B2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -13,7 +14,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$357</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -1766,7 +1767,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1827,7 +1828,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1844,7 +1845,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1919,6 +1920,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1954,6 +1972,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2129,20 +2164,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="A246" sqref="A246"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
     <col min="6" max="6" width="81.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5966,7 +6001,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F357"/>
+  <autoFilter ref="A1:F357" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
exercices modules 3 achieved
</commit_message>
<xml_diff>
--- a/Courses/Courses/course_projects/Data/module_3/meta_data.xlsx
+++ b/Courses/Courses/course_projects/Data/module_3/meta_data.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{735A848A-67B9-4B3D-9E53-0FBF4BCCD8B2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +13,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$357</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1767,7 +1766,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1828,7 +1827,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1845,7 +1844,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1920,23 +1919,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1972,23 +1954,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2164,14 +2129,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F357"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D281" sqref="D281"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
@@ -3503,7 +3468,7 @@
         <v>461</v>
       </c>
       <c r="C133" t="s">
-        <v>462</v>
+        <v>420</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -5119,7 +5084,7 @@
         <v>520</v>
       </c>
       <c r="C281" t="s">
-        <v>462</v>
+        <v>420</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
@@ -6001,7 +5966,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F357" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F357"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>